<commit_message>
Gallery, countdown, location finished
</commit_message>
<xml_diff>
--- a/src/assets/bd/invitados.xlsx
+++ b/src/assets/bd/invitados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\OneDrive\Documentos\0_Invitacion_boda\invitacion-boda\src\assets\bd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D40FCDD-CDD5-42E5-BED9-805BC1A80E0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29EDC54F-2855-4837-B8FE-273DFD633EA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0E51308E-29DF-4646-B0C1-41E0F87AEFC9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>Laura Eugenia Gómez García</t>
   </si>
@@ -165,12 +165,6 @@
   </si>
   <si>
     <t>Esposo</t>
-  </si>
-  <si>
-    <t>Mónica Ávila</t>
-  </si>
-  <si>
-    <t>Padrino</t>
   </si>
   <si>
     <t>Novia, bebe</t>
@@ -620,10 +614,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC699A7F-9C7E-40BA-B728-D3157C7F64CC}">
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -650,13 +644,13 @@
         <v>33</v>
       </c>
       <c r="E1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" t="s">
         <v>50</v>
-      </c>
-      <c r="F1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -833,7 +827,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -869,7 +863,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B19">
         <v>2</v>
@@ -936,7 +930,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -967,7 +961,7 @@
         <v>0</v>
       </c>
       <c r="D26" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -994,7 +988,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B29">
         <v>2</v>
@@ -1033,16 +1027,16 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="B32">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C32" s="1" t="b">
         <v>0</v>
       </c>
       <c r="D32" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1050,7 +1044,7 @@
         <v>54</v>
       </c>
       <c r="B33">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C33" s="1" t="b">
         <v>0</v>
@@ -1061,39 +1055,25 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>55</v>
+      </c>
+      <c r="B34">
+        <v>2</v>
+      </c>
+      <c r="C34" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D34" t="s">
         <v>56</v>
       </c>
-      <c r="B34">
-        <v>2</v>
-      </c>
-      <c r="C34" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D34" t="s">
-        <v>55</v>
-      </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="A35" s="2" t="s">
         <v>57</v>
       </c>
       <c r="B35">
-        <v>2</v>
-      </c>
-      <c r="C35" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D35" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B36">
-        <f>SUM(B2:B35)</f>
-        <v>58</v>
+        <f>SUM(B2:B34)</f>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>